<commit_message>
Add GPS functionality with continuous reading and location retrieval
</commit_message>
<xml_diff>
--- a/Raspberry Pi GPIO.xlsx
+++ b/Raspberry Pi GPIO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\GitHub\autonomous_mower\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C73562A-4E17-4FF4-A967-117BC1CCDE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAAC759-85D4-437D-9C20-2A622C13B5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{306695F8-C1B8-4336-AFCE-81902104763D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{306695F8-C1B8-4336-AFCE-81902104763D}"/>
   </bookViews>
   <sheets>
     <sheet name="Pi 4 Pin Function List" sheetId="1" r:id="rId1"/>
@@ -3198,7 +3198,7 @@
   <dimension ref="B2:L24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3473,7 +3473,9 @@
       <c r="L13" s="15"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
+      <c r="B14" s="10" t="s">
+        <v>290</v>
+      </c>
       <c r="C14" s="10" t="s">
         <v>285</v>
       </c>
@@ -3517,7 +3519,9 @@
       <c r="H15" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="I15" s="10"/>
+      <c r="I15" s="10" t="s">
+        <v>291</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="14"/>
     </row>
@@ -3544,9 +3548,7 @@
       <c r="K16" s="14"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
-        <v>291</v>
-      </c>
+      <c r="B17" s="10"/>
       <c r="C17" s="10" t="s">
         <v>280</v>
       </c>
@@ -3567,9 +3569,7 @@
       <c r="H17" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="I17" s="10" t="s">
-        <v>290</v>
-      </c>
+      <c r="I17" s="10"/>
       <c r="J17" s="1"/>
       <c r="K17" s="14"/>
     </row>

</xml_diff>